<commit_message>
updated BOM for latest version 3.3C of board
</commit_message>
<xml_diff>
--- a/BOM/T962A_Controller_TFT_BOM.xlsx
+++ b/BOM/T962A_Controller_TFT_BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="345">
   <si>
     <t>Manufacturer Part Number</t>
   </si>
@@ -103,25 +103,10 @@
     <t>Not Available</t>
   </si>
   <si>
-    <t>TC50L5I32K7680</t>
-  </si>
-  <si>
-    <t>CTS-Frequency Controls</t>
-  </si>
-  <si>
-    <t>CTX1185CT-ND</t>
-  </si>
-  <si>
     <t>Cut Tape (CT)</t>
   </si>
   <si>
-    <t>$2.18</t>
-  </si>
-  <si>
     <t>13 Weeks</t>
-  </si>
-  <si>
-    <t>XTAL OSC XO 32.7680KHZ CMOS</t>
   </si>
   <si>
     <t>REACH Unaffected</t>
@@ -1084,6 +1069,48 @@
   </si>
   <si>
     <t>5.0" TFT w/NO bracket</t>
+  </si>
+  <si>
+    <t>644-1386-1-ND</t>
+  </si>
+  <si>
+    <t>CRYSTAL 32.768KHZ 6PF SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 Weeks </t>
+  </si>
+  <si>
+    <t>NDK America, Inc</t>
+  </si>
+  <si>
+    <t>NX3215SA-32.768KHZ-EXS00A-MU00525</t>
+  </si>
+  <si>
+    <t>311-1737-1-ND</t>
+  </si>
+  <si>
+    <t>CC0603BRNPO9BN1R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 Weeks </t>
+  </si>
+  <si>
+    <t>CAP CER 1.5PF 50V C0G/NPO 0603</t>
+  </si>
+  <si>
+    <t>BAT-HLD-001-ND</t>
+  </si>
+  <si>
+    <t>Linx Technologies Inc</t>
+  </si>
+  <si>
+    <t>BAT-HLD-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Weeks </t>
+  </si>
+  <si>
+    <t>BATTERY RETAINER COIN 20MM SMD</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1231,6 +1258,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1525,10 +1554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q80"/>
+  <dimension ref="A1:Q82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1658,13 +1687,13 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -1673,7 +1702,7 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
@@ -1685,16 +1714,16 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="J3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="K3">
         <v>55048</v>
       </c>
       <c r="L3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="N3" t="s">
         <v>26</v>
@@ -1703,7 +1732,7 @@
         <v>27</v>
       </c>
       <c r="P3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q3" t="s">
         <v>20</v>
@@ -1711,13 +1740,13 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="2" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B4" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C4" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -1726,7 +1755,7 @@
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
@@ -1738,16 +1767,16 @@
         <v>0.25</v>
       </c>
       <c r="J4" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="K4">
         <v>2448</v>
       </c>
       <c r="L4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="N4" t="s">
         <v>26</v>
@@ -1756,7 +1785,7 @@
         <v>27</v>
       </c>
       <c r="P4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q4" t="s">
         <v>20</v>
@@ -1764,14 +1793,14 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="2" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C5" t="s">
         <v>288</v>
       </c>
-      <c r="C5" t="s">
-        <v>293</v>
-      </c>
       <c r="D5" t="s">
         <v>20</v>
       </c>
@@ -1779,7 +1808,7 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G5" t="s">
         <v>22</v>
@@ -1791,16 +1820,16 @@
         <v>0.27</v>
       </c>
       <c r="J5" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="K5">
         <v>2584</v>
       </c>
       <c r="L5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="M5" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="N5" t="s">
         <v>26</v>
@@ -1809,7 +1838,7 @@
         <v>27</v>
       </c>
       <c r="P5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q5" t="s">
         <v>20</v>
@@ -1817,13 +1846,13 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -1832,7 +1861,7 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
         <v>22</v>
@@ -1844,16 +1873,16 @@
         <v>0.5</v>
       </c>
       <c r="J6" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="K6">
         <v>2022</v>
       </c>
       <c r="L6" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="M6" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="N6" t="s">
         <v>26</v>
@@ -1870,13 +1899,13 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B7" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C7" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
@@ -1885,7 +1914,7 @@
         <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
         <v>22</v>
@@ -1897,7 +1926,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="J7" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K7">
         <v>56557</v>
@@ -1906,7 +1935,7 @@
         <v>28</v>
       </c>
       <c r="M7" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="N7" t="s">
         <v>26</v>
@@ -1915,21 +1944,21 @@
         <v>27</v>
       </c>
       <c r="P7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C8" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
@@ -1938,7 +1967,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
         <v>22</v>
@@ -1950,16 +1979,16 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="J8" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="K8">
         <v>720992</v>
       </c>
       <c r="L8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="M8" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="N8" t="s">
         <v>26</v>
@@ -1968,7 +1997,7 @@
         <v>27</v>
       </c>
       <c r="P8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q8" t="s">
         <v>20</v>
@@ -1976,13 +2005,13 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C9" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -1991,7 +2020,7 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G9" t="s">
         <v>22</v>
@@ -2003,16 +2032,16 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="J9" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="K9">
         <v>545099</v>
       </c>
       <c r="L9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="M9" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="N9" t="s">
         <v>26</v>
@@ -2021,21 +2050,21 @@
         <v>27</v>
       </c>
       <c r="P9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B10" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
@@ -2044,7 +2073,7 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
         <v>22</v>
@@ -2056,7 +2085,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="J10" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="K10">
         <v>24491685</v>
@@ -2065,7 +2094,7 @@
         <v>28</v>
       </c>
       <c r="M10" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="N10" t="s">
         <v>26</v>
@@ -2082,13 +2111,13 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C11" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
@@ -2097,7 +2126,7 @@
         <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G11" t="s">
         <v>22</v>
@@ -2109,7 +2138,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="J11" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="K11">
         <v>402823</v>
@@ -2118,7 +2147,7 @@
         <v>28</v>
       </c>
       <c r="M11" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="N11" t="s">
         <v>26</v>
@@ -2130,18 +2159,18 @@
         <v>28</v>
       </c>
       <c r="Q11" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B12" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C12" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -2150,7 +2179,7 @@
         <v>20</v>
       </c>
       <c r="F12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s">
         <v>22</v>
@@ -2162,7 +2191,7 @@
         <v>0.216</v>
       </c>
       <c r="J12" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="K12">
         <v>4440420</v>
@@ -2171,7 +2200,7 @@
         <v>28</v>
       </c>
       <c r="M12" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="N12" t="s">
         <v>26</v>
@@ -2188,13 +2217,13 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B13" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
@@ -2203,7 +2232,7 @@
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G13" t="s">
         <v>22</v>
@@ -2215,7 +2244,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="J13" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="K13">
         <v>3131933</v>
@@ -2224,7 +2253,7 @@
         <v>28</v>
       </c>
       <c r="M13" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="N13" t="s">
         <v>26</v>
@@ -2233,21 +2262,21 @@
         <v>27</v>
       </c>
       <c r="P13" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C14" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -2256,7 +2285,7 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G14" t="s">
         <v>22</v>
@@ -2268,7 +2297,7 @@
         <v>0.155</v>
       </c>
       <c r="J14" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="K14">
         <v>475706</v>
@@ -2277,7 +2306,7 @@
         <v>28</v>
       </c>
       <c r="M14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="N14" t="s">
         <v>26</v>
@@ -2286,7 +2315,7 @@
         <v>27</v>
       </c>
       <c r="P14" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q14" t="s">
         <v>20</v>
@@ -2294,13 +2323,13 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="2" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B15" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C15" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D15" t="s">
         <v>20</v>
@@ -2309,7 +2338,7 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G15" t="s">
         <v>22</v>
@@ -2321,7 +2350,7 @@
         <v>0.37</v>
       </c>
       <c r="J15" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="K15">
         <v>295747</v>
@@ -2330,7 +2359,7 @@
         <v>28</v>
       </c>
       <c r="M15" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="N15" t="s">
         <v>26</v>
@@ -2347,13 +2376,13 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
@@ -2362,10 +2391,10 @@
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H16">
         <v>4</v>
@@ -2374,7 +2403,7 @@
         <v>1.06</v>
       </c>
       <c r="J16" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="K16">
         <v>929013</v>
@@ -2383,7 +2412,7 @@
         <v>28</v>
       </c>
       <c r="M16" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="N16" t="s">
         <v>26</v>
@@ -2400,13 +2429,13 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
@@ -2415,7 +2444,7 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s">
         <v>22</v>
@@ -2427,16 +2456,16 @@
         <v>2.94</v>
       </c>
       <c r="J17" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="K17">
         <v>23875</v>
       </c>
       <c r="L17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M17" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="N17" t="s">
         <v>26</v>
@@ -2445,7 +2474,7 @@
         <v>27</v>
       </c>
       <c r="P17" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q17" t="s">
         <v>20</v>
@@ -2453,13 +2482,13 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="2" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -2468,7 +2497,7 @@
         <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G18" t="s">
         <v>22</v>
@@ -2480,16 +2509,16 @@
         <v>0.99</v>
       </c>
       <c r="J18" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="K18">
         <v>15549</v>
       </c>
       <c r="L18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="M18" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="N18" t="s">
         <v>26</v>
@@ -2498,7 +2527,7 @@
         <v>27</v>
       </c>
       <c r="P18" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q18" t="s">
         <v>20</v>
@@ -2509,10 +2538,10 @@
         <v>61302411121</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
@@ -2521,7 +2550,7 @@
         <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="G19" t="s">
         <v>22</v>
@@ -2533,16 +2562,16 @@
         <v>1.23</v>
       </c>
       <c r="J19" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="K19">
         <v>717</v>
       </c>
       <c r="L19" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="M19" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="N19" t="s">
         <v>26</v>
@@ -2551,7 +2580,7 @@
         <v>27</v>
       </c>
       <c r="P19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q19" t="s">
         <v>20</v>
@@ -2559,14 +2588,14 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="2" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B20" t="s">
+        <v>311</v>
+      </c>
+      <c r="C20" t="s">
         <v>316</v>
       </c>
-      <c r="C20" t="s">
-        <v>321</v>
-      </c>
       <c r="D20" t="s">
         <v>20</v>
       </c>
@@ -2574,7 +2603,7 @@
         <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G20" t="s">
         <v>22</v>
@@ -2586,16 +2615,16 @@
         <v>0.15</v>
       </c>
       <c r="J20" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="K20">
         <v>193381</v>
       </c>
       <c r="L20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="M20" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="N20" t="s">
         <v>26</v>
@@ -2607,18 +2636,18 @@
         <v>28</v>
       </c>
       <c r="Q20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="2" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
@@ -2627,7 +2656,7 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="G21" t="s">
         <v>22</v>
@@ -2639,16 +2668,16 @@
         <v>0.27</v>
       </c>
       <c r="J21" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="K21">
         <v>20765</v>
       </c>
       <c r="L21" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="M21" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="N21" t="s">
         <v>26</v>
@@ -2657,7 +2686,7 @@
         <v>27</v>
       </c>
       <c r="P21" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q21" t="s">
         <v>20</v>
@@ -2665,13 +2694,13 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="2" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D22" t="s">
         <v>20</v>
@@ -2680,7 +2709,7 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G22" t="s">
         <v>22</v>
@@ -2692,16 +2721,16 @@
         <v>0.38</v>
       </c>
       <c r="J22" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="K22">
         <v>18308</v>
       </c>
       <c r="L22" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M22" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="N22" t="s">
         <v>26</v>
@@ -2710,7 +2739,7 @@
         <v>27</v>
       </c>
       <c r="P22" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q22" t="s">
         <v>20</v>
@@ -2718,13 +2747,13 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="2" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B23" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C23" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D23" t="s">
         <v>20</v>
@@ -2733,7 +2762,7 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G23" t="s">
         <v>22</v>
@@ -2745,16 +2774,16 @@
         <v>0.21</v>
       </c>
       <c r="J23" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="K23">
         <v>182142</v>
       </c>
       <c r="L23" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="M23" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="N23" t="s">
         <v>26</v>
@@ -2766,18 +2795,18 @@
         <v>28</v>
       </c>
       <c r="Q23" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
@@ -2786,7 +2815,7 @@
         <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G24" t="s">
         <v>22</v>
@@ -2798,7 +2827,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="J24" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="K24">
         <v>34621</v>
@@ -2807,7 +2836,7 @@
         <v>24</v>
       </c>
       <c r="M24" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="N24" t="s">
         <v>26</v>
@@ -2816,21 +2845,21 @@
         <v>27</v>
       </c>
       <c r="P24" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q24" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D25" t="s">
         <v>20</v>
@@ -2839,7 +2868,7 @@
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G25" t="s">
         <v>22</v>
@@ -2851,16 +2880,16 @@
         <v>1.24</v>
       </c>
       <c r="J25" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K25">
         <v>14494</v>
       </c>
       <c r="L25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="M25" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="N25" t="s">
         <v>26</v>
@@ -2872,18 +2901,18 @@
         <v>28</v>
       </c>
       <c r="Q25" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
         <v>20</v>
@@ -2892,7 +2921,7 @@
         <v>20</v>
       </c>
       <c r="F26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G26" t="s">
         <v>22</v>
@@ -2904,16 +2933,16 @@
         <v>0.39</v>
       </c>
       <c r="J26" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="K26">
         <v>34215</v>
       </c>
       <c r="L26" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="M26" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="N26" t="s">
         <v>26</v>
@@ -2922,21 +2951,21 @@
         <v>27</v>
       </c>
       <c r="P26" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q26" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B27" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D27" t="s">
         <v>20</v>
@@ -2945,7 +2974,7 @@
         <v>20</v>
       </c>
       <c r="F27" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G27" t="s">
         <v>22</v>
@@ -2957,25 +2986,25 @@
         <v>0.54</v>
       </c>
       <c r="J27" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="K27">
         <v>34505</v>
       </c>
       <c r="L27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M27" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="N27" t="s">
         <v>26</v>
       </c>
       <c r="O27" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="P27" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q27" t="s">
         <v>20</v>
@@ -2983,13 +3012,13 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C28" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D28" t="s">
         <v>20</v>
@@ -2998,7 +3027,7 @@
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G28" t="s">
         <v>22</v>
@@ -3010,16 +3039,16 @@
         <v>0.11</v>
       </c>
       <c r="J28" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="K28">
         <v>573851</v>
       </c>
       <c r="L28" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M28" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="N28" t="s">
         <v>26</v>
@@ -3028,7 +3057,7 @@
         <v>27</v>
       </c>
       <c r="P28" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q28" t="s">
         <v>20</v>
@@ -3036,14 +3065,14 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" t="s">
         <v>134</v>
       </c>
-      <c r="C29" t="s">
-        <v>139</v>
-      </c>
       <c r="D29" t="s">
         <v>20</v>
       </c>
@@ -3051,7 +3080,7 @@
         <v>20</v>
       </c>
       <c r="F29" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G29" t="s">
         <v>22</v>
@@ -3063,7 +3092,7 @@
         <v>0.76</v>
       </c>
       <c r="J29" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K29">
         <v>2523</v>
@@ -3072,7 +3101,7 @@
         <v>24</v>
       </c>
       <c r="M29" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="N29" t="s">
         <v>26</v>
@@ -3084,18 +3113,18 @@
         <v>28</v>
       </c>
       <c r="Q29" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D30" t="s">
         <v>20</v>
@@ -3104,7 +3133,7 @@
         <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G30" t="s">
         <v>22</v>
@@ -3116,16 +3145,16 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="J30" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="K30">
         <v>43390</v>
       </c>
       <c r="L30" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="M30" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="N30" t="s">
         <v>26</v>
@@ -3145,10 +3174,10 @@
         <v>74438357056</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C31" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D31" t="s">
         <v>20</v>
@@ -3157,7 +3186,7 @@
         <v>20</v>
       </c>
       <c r="F31" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G31" t="s">
         <v>22</v>
@@ -3169,16 +3198,16 @@
         <v>1.58</v>
       </c>
       <c r="J31" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="K31">
         <v>703</v>
       </c>
       <c r="L31" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="M31" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="N31" t="s">
         <v>26</v>
@@ -3187,7 +3216,7 @@
         <v>27</v>
       </c>
       <c r="P31" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q31" t="s">
         <v>20</v>
@@ -3198,10 +3227,10 @@
         <v>3527</v>
       </c>
       <c r="B32" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C32" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D32" t="s">
         <v>20</v>
@@ -3210,7 +3239,7 @@
         <v>20</v>
       </c>
       <c r="F32" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="G32" t="s">
         <v>22</v>
@@ -3222,16 +3251,16 @@
         <v>1.36</v>
       </c>
       <c r="J32" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="K32">
         <v>4061</v>
       </c>
       <c r="L32" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="M32" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="N32" t="s">
         <v>26</v>
@@ -3240,7 +3269,7 @@
         <v>27</v>
       </c>
       <c r="P32" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q32" t="s">
         <v>20</v>
@@ -3248,13 +3277,13 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
         <v>20</v>
@@ -3263,7 +3292,7 @@
         <v>20</v>
       </c>
       <c r="F33" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G33" t="s">
         <v>22</v>
@@ -3275,16 +3304,16 @@
         <v>0.45</v>
       </c>
       <c r="J33" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="K33">
         <v>14857</v>
       </c>
       <c r="L33" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="M33" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="N33" t="s">
         <v>26</v>
@@ -3293,7 +3322,7 @@
         <v>27</v>
       </c>
       <c r="P33" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q33" t="s">
         <v>20</v>
@@ -3301,13 +3330,13 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D34" t="s">
         <v>20</v>
@@ -3316,7 +3345,7 @@
         <v>20</v>
       </c>
       <c r="F34" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G34" t="s">
         <v>22</v>
@@ -3328,16 +3357,16 @@
         <v>6.52</v>
       </c>
       <c r="J34" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K34">
         <v>7645</v>
       </c>
       <c r="L34" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="M34" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="N34" t="s">
         <v>26</v>
@@ -3346,7 +3375,7 @@
         <v>27</v>
       </c>
       <c r="P34" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q34" t="s">
         <v>20</v>
@@ -3354,13 +3383,13 @@
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
         <v>20</v>
@@ -3381,16 +3410,16 @@
         <v>14.15</v>
       </c>
       <c r="J35" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K35">
         <v>392</v>
       </c>
       <c r="L35" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="M35" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="N35" t="s">
         <v>26</v>
@@ -3399,21 +3428,21 @@
         <v>27</v>
       </c>
       <c r="P35" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q35" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:17">
       <c r="A36" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D36" t="s">
         <v>20</v>
@@ -3422,7 +3451,7 @@
         <v>20</v>
       </c>
       <c r="F36" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G36" t="s">
         <v>22</v>
@@ -3434,16 +3463,16 @@
         <v>0.99</v>
       </c>
       <c r="J36" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K36">
         <v>13246</v>
       </c>
       <c r="L36" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="M36" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="N36" t="s">
         <v>26</v>
@@ -3452,7 +3481,7 @@
         <v>27</v>
       </c>
       <c r="P36" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q36" t="s">
         <v>20</v>
@@ -3460,13 +3489,13 @@
     </row>
     <row r="37" spans="1:17">
       <c r="A37" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D37" t="s">
         <v>20</v>
@@ -3487,16 +3516,16 @@
         <v>17.18</v>
       </c>
       <c r="J37" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="K37">
         <v>459</v>
       </c>
       <c r="L37" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M37" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="N37" t="s">
         <v>26</v>
@@ -3505,7 +3534,7 @@
         <v>27</v>
       </c>
       <c r="P37" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q37" t="s">
         <v>20</v>
@@ -3513,13 +3542,13 @@
     </row>
     <row r="38" spans="1:17">
       <c r="A38" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D38" t="s">
         <v>20</v>
@@ -3528,7 +3557,7 @@
         <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G38" t="s">
         <v>22</v>
@@ -3540,16 +3569,16 @@
         <v>1.6</v>
       </c>
       <c r="J38" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K38">
         <v>26890</v>
       </c>
       <c r="L38" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="M38" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="N38" t="s">
         <v>26</v>
@@ -3558,7 +3587,7 @@
         <v>27</v>
       </c>
       <c r="P38" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q38" t="s">
         <v>20</v>
@@ -3566,13 +3595,13 @@
     </row>
     <row r="39" spans="1:17">
       <c r="A39" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D39" t="s">
         <v>20</v>
@@ -3581,7 +3610,7 @@
         <v>20</v>
       </c>
       <c r="F39" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G39" t="s">
         <v>22</v>
@@ -3593,16 +3622,16 @@
         <v>0.42</v>
       </c>
       <c r="J39" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K39">
         <v>447</v>
       </c>
       <c r="L39" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="M39" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="N39" t="s">
         <v>26</v>
@@ -3611,7 +3640,7 @@
         <v>27</v>
       </c>
       <c r="P39" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q39" t="s">
         <v>20</v>
@@ -3619,13 +3648,13 @@
     </row>
     <row r="40" spans="1:17">
       <c r="A40" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D40" t="s">
         <v>20</v>
@@ -3634,7 +3663,7 @@
         <v>20</v>
       </c>
       <c r="F40" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G40" t="s">
         <v>22</v>
@@ -3646,7 +3675,7 @@
         <v>0.45</v>
       </c>
       <c r="J40" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="K40">
         <v>21179</v>
@@ -3655,7 +3684,7 @@
         <v>24</v>
       </c>
       <c r="M40" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="N40" t="s">
         <v>26</v>
@@ -3664,7 +3693,7 @@
         <v>27</v>
       </c>
       <c r="P40" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q40" t="s">
         <v>20</v>
@@ -3672,13 +3701,13 @@
     </row>
     <row r="41" spans="1:17">
       <c r="A41" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D41" t="s">
         <v>20</v>
@@ -3687,7 +3716,7 @@
         <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G41" t="s">
         <v>22</v>
@@ -3699,16 +3728,16 @@
         <v>0.34</v>
       </c>
       <c r="J41" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K41">
         <v>145200</v>
       </c>
       <c r="L41" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M41" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="N41" t="s">
         <v>26</v>
@@ -3717,21 +3746,21 @@
         <v>27</v>
       </c>
       <c r="P41" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q41" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:17">
       <c r="A42" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D42" t="s">
         <v>20</v>
@@ -3740,7 +3769,7 @@
         <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G42" t="s">
         <v>22</v>
@@ -3752,7 +3781,7 @@
         <v>1.44</v>
       </c>
       <c r="J42" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="K42">
         <v>2803</v>
@@ -3761,7 +3790,7 @@
         <v>28</v>
       </c>
       <c r="M42" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="N42" t="s">
         <v>26</v>
@@ -3773,18 +3802,18 @@
         <v>28</v>
       </c>
       <c r="Q42" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:17">
       <c r="A43" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B43" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C43" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D43" t="s">
         <v>20</v>
@@ -3793,7 +3822,7 @@
         <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G43" t="s">
         <v>22</v>
@@ -3805,7 +3834,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="J43" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="K43">
         <v>40499</v>
@@ -3814,7 +3843,7 @@
         <v>28</v>
       </c>
       <c r="M43" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="N43" t="s">
         <v>26</v>
@@ -3831,13 +3860,13 @@
     </row>
     <row r="44" spans="1:17">
       <c r="A44" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B44" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C44" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D44" t="s">
         <v>20</v>
@@ -3846,7 +3875,7 @@
         <v>20</v>
       </c>
       <c r="F44" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G44" t="s">
         <v>22</v>
@@ -3858,16 +3887,16 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="J44" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K44">
         <v>22521</v>
       </c>
       <c r="L44" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M44" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="N44" t="s">
         <v>26</v>
@@ -3876,7 +3905,7 @@
         <v>27</v>
       </c>
       <c r="P44" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q44" t="s">
         <v>20</v>
@@ -3884,13 +3913,13 @@
     </row>
     <row r="45" spans="1:17">
       <c r="A45" s="2" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C45" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D45" t="s">
         <v>20</v>
@@ -3899,7 +3928,7 @@
         <v>20</v>
       </c>
       <c r="F45" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G45" t="s">
         <v>22</v>
@@ -3911,16 +3940,16 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="J45" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K45">
         <v>682651</v>
       </c>
       <c r="L45" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M45" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="N45" t="s">
         <v>26</v>
@@ -3929,7 +3958,7 @@
         <v>27</v>
       </c>
       <c r="P45" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q45" t="s">
         <v>20</v>
@@ -3937,13 +3966,13 @@
     </row>
     <row r="46" spans="1:17">
       <c r="A46" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B46" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C46" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D46" t="s">
         <v>20</v>
@@ -3952,7 +3981,7 @@
         <v>20</v>
       </c>
       <c r="F46" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G46" t="s">
         <v>22</v>
@@ -3964,16 +3993,16 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="J46" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="K46">
         <v>4468</v>
       </c>
       <c r="L46" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M46" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="N46" t="s">
         <v>26</v>
@@ -3982,7 +4011,7 @@
         <v>27</v>
       </c>
       <c r="P46" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q46" t="s">
         <v>20</v>
@@ -3990,13 +4019,13 @@
     </row>
     <row r="47" spans="1:17">
       <c r="A47" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B47" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C47" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D47" t="s">
         <v>20</v>
@@ -4005,7 +4034,7 @@
         <v>20</v>
       </c>
       <c r="F47" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G47" t="s">
         <v>22</v>
@@ -4017,16 +4046,16 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="J47" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K47">
         <v>29531752</v>
       </c>
       <c r="L47" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M47" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="N47" t="s">
         <v>26</v>
@@ -4035,21 +4064,21 @@
         <v>27</v>
       </c>
       <c r="P47" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q47" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:17">
       <c r="A48" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B48" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C48" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D48" t="s">
         <v>20</v>
@@ -4058,7 +4087,7 @@
         <v>20</v>
       </c>
       <c r="F48" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G48" t="s">
         <v>22</v>
@@ -4070,16 +4099,16 @@
         <v>0.06</v>
       </c>
       <c r="J48" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="K48">
         <v>5268022</v>
       </c>
       <c r="L48" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M48" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="N48" t="s">
         <v>26</v>
@@ -4088,21 +4117,21 @@
         <v>27</v>
       </c>
       <c r="P48" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q48" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:17">
       <c r="A49" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B49" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C49" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D49" t="s">
         <v>20</v>
@@ -4111,7 +4140,7 @@
         <v>20</v>
       </c>
       <c r="F49" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G49" t="s">
         <v>22</v>
@@ -4123,16 +4152,16 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="J49" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K49">
         <v>1706629</v>
       </c>
       <c r="L49" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M49" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N49" t="s">
         <v>26</v>
@@ -4141,21 +4170,21 @@
         <v>27</v>
       </c>
       <c r="P49" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q49" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:17">
       <c r="A50" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B50" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D50" t="s">
         <v>20</v>
@@ -4164,7 +4193,7 @@
         <v>20</v>
       </c>
       <c r="F50" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G50" t="s">
         <v>22</v>
@@ -4176,16 +4205,16 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="J50" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K50">
         <v>28427723</v>
       </c>
       <c r="L50" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M50" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="N50" t="s">
         <v>26</v>
@@ -4194,21 +4223,21 @@
         <v>27</v>
       </c>
       <c r="P50" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q50" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:17">
       <c r="A51" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B51" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C51" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D51" t="s">
         <v>20</v>
@@ -4217,7 +4246,7 @@
         <v>20</v>
       </c>
       <c r="F51" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G51" t="s">
         <v>22</v>
@@ -4229,16 +4258,16 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="J51" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K51">
         <v>211572</v>
       </c>
       <c r="L51" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M51" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="N51" t="s">
         <v>26</v>
@@ -4247,21 +4276,21 @@
         <v>27</v>
       </c>
       <c r="P51" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q51" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:17">
       <c r="A52" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B52" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C52" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D52" t="s">
         <v>20</v>
@@ -4270,7 +4299,7 @@
         <v>20</v>
       </c>
       <c r="F52" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G52" t="s">
         <v>22</v>
@@ -4282,16 +4311,16 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="J52" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K52">
         <v>6715917</v>
       </c>
       <c r="L52" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M52" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="N52" t="s">
         <v>26</v>
@@ -4300,21 +4329,21 @@
         <v>27</v>
       </c>
       <c r="P52" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q52" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:17">
       <c r="A53" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B53" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C53" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D53" t="s">
         <v>20</v>
@@ -4323,7 +4352,7 @@
         <v>20</v>
       </c>
       <c r="F53" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G53" t="s">
         <v>22</v>
@@ -4335,16 +4364,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="J53" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="K53">
         <v>73339</v>
       </c>
       <c r="L53" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M53" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="N53" t="s">
         <v>26</v>
@@ -4353,7 +4382,7 @@
         <v>27</v>
       </c>
       <c r="P53" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q53" t="s">
         <v>20</v>
@@ -4361,13 +4390,13 @@
     </row>
     <row r="54" spans="1:17">
       <c r="A54" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B54" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C54" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D54" t="s">
         <v>20</v>
@@ -4376,7 +4405,7 @@
         <v>20</v>
       </c>
       <c r="F54" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G54" t="s">
         <v>22</v>
@@ -4388,16 +4417,16 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="J54" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K54">
         <v>113718</v>
       </c>
       <c r="L54" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M54" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="N54" t="s">
         <v>26</v>
@@ -4406,21 +4435,21 @@
         <v>27</v>
       </c>
       <c r="P54" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q54" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="1:17">
       <c r="A55" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B55" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C55" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D55" t="s">
         <v>20</v>
@@ -4429,7 +4458,7 @@
         <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G55" t="s">
         <v>22</v>
@@ -4441,16 +4470,16 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="J55" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K55">
         <v>896474</v>
       </c>
       <c r="L55" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M55" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="N55" t="s">
         <v>26</v>
@@ -4459,21 +4488,21 @@
         <v>27</v>
       </c>
       <c r="P55" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q55" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:17">
       <c r="A56" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B56" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C56" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D56" t="s">
         <v>20</v>
@@ -4482,7 +4511,7 @@
         <v>20</v>
       </c>
       <c r="F56" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G56" t="s">
         <v>22</v>
@@ -4494,16 +4523,16 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="J56" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K56">
         <v>1773289</v>
       </c>
       <c r="L56" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M56" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="N56" t="s">
         <v>26</v>
@@ -4512,21 +4541,21 @@
         <v>27</v>
       </c>
       <c r="P56" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q56" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:17">
       <c r="A57" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B57" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C57" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D57" t="s">
         <v>20</v>
@@ -4535,7 +4564,7 @@
         <v>20</v>
       </c>
       <c r="F57" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G57" t="s">
         <v>22</v>
@@ -4547,16 +4576,16 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="J57" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="K57">
         <v>344004</v>
       </c>
       <c r="L57" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M57" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="N57" t="s">
         <v>26</v>
@@ -4565,21 +4594,21 @@
         <v>27</v>
       </c>
       <c r="P57" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q57" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:17">
       <c r="A58" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B58" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C58" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D58" t="s">
         <v>20</v>
@@ -4588,7 +4617,7 @@
         <v>20</v>
       </c>
       <c r="F58" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G58" t="s">
         <v>22</v>
@@ -4600,16 +4629,16 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="J58" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K58">
         <v>1491680</v>
       </c>
       <c r="L58" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M58" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="N58" t="s">
         <v>26</v>
@@ -4618,21 +4647,21 @@
         <v>27</v>
       </c>
       <c r="P58" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q58" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:17">
       <c r="A59" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B59" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C59" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D59" t="s">
         <v>20</v>
@@ -4641,7 +4670,7 @@
         <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G59" t="s">
         <v>22</v>
@@ -4653,16 +4682,16 @@
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="J59" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="K59">
         <v>2938013</v>
       </c>
       <c r="L59" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M59" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="N59" t="s">
         <v>26</v>
@@ -4671,21 +4700,21 @@
         <v>27</v>
       </c>
       <c r="P59" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q59" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:17">
       <c r="A60" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B60" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C60" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D60" t="s">
         <v>20</v>
@@ -4694,7 +4723,7 @@
         <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G60" t="s">
         <v>22</v>
@@ -4706,16 +4735,16 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="J60" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K60">
         <v>772722</v>
       </c>
       <c r="L60" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M60" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="N60" t="s">
         <v>26</v>
@@ -4724,21 +4753,21 @@
         <v>27</v>
       </c>
       <c r="P60" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q60" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:17">
       <c r="A61" s="2" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B61" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C61" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D61" t="s">
         <v>20</v>
@@ -4747,7 +4776,7 @@
         <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G61" t="s">
         <v>22</v>
@@ -4759,16 +4788,16 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="J61" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K61">
         <v>7910116</v>
       </c>
       <c r="L61" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M61" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="N61" t="s">
         <v>26</v>
@@ -4777,21 +4806,21 @@
         <v>27</v>
       </c>
       <c r="P61" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q61" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" spans="1:17">
       <c r="A62" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B62" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C62" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D62" t="s">
         <v>20</v>
@@ -4800,7 +4829,7 @@
         <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G62" t="s">
         <v>22</v>
@@ -4812,16 +4841,16 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="J62" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="K62">
         <v>2270418</v>
       </c>
       <c r="L62" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M62" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="N62" t="s">
         <v>26</v>
@@ -4830,21 +4859,21 @@
         <v>27</v>
       </c>
       <c r="P62" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q62" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="63" spans="1:17">
       <c r="A63" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B63" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C63" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D63" t="s">
         <v>20</v>
@@ -4853,7 +4882,7 @@
         <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G63" t="s">
         <v>22</v>
@@ -4865,16 +4894,16 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="J63" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K63">
         <v>692895</v>
       </c>
       <c r="L63" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M63" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="N63" t="s">
         <v>26</v>
@@ -4883,21 +4912,21 @@
         <v>27</v>
       </c>
       <c r="P63" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q63" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:17">
       <c r="A64" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B64" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C64" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D64" t="s">
         <v>20</v>
@@ -4906,7 +4935,7 @@
         <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G64" t="s">
         <v>22</v>
@@ -4918,16 +4947,16 @@
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="J64" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="K64">
         <v>685270</v>
       </c>
       <c r="L64" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M64" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="N64" t="s">
         <v>26</v>
@@ -4936,21 +4965,21 @@
         <v>27</v>
       </c>
       <c r="P64" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q64" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="65" spans="1:17">
       <c r="A65" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B65" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C65" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D65" t="s">
         <v>20</v>
@@ -4959,7 +4988,7 @@
         <v>20</v>
       </c>
       <c r="F65" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G65" t="s">
         <v>22</v>
@@ -4971,16 +5000,16 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="J65" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K65">
         <v>231228</v>
       </c>
       <c r="L65" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="M65" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="N65" t="s">
         <v>26</v>
@@ -4989,21 +5018,21 @@
         <v>27</v>
       </c>
       <c r="P65" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q65" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="66" spans="1:17">
       <c r="A66" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B66" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C66" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D66" t="s">
         <v>20</v>
@@ -5012,7 +5041,7 @@
         <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G66" t="s">
         <v>22</v>
@@ -5024,16 +5053,16 @@
         <v>0.73</v>
       </c>
       <c r="J66" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="K66">
         <v>20752</v>
       </c>
       <c r="L66" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="M66" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="N66" t="s">
         <v>26</v>
@@ -5042,21 +5071,21 @@
         <v>27</v>
       </c>
       <c r="P66" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q66" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:17">
       <c r="A67" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B67" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C67" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D67" t="s">
         <v>20</v>
@@ -5065,7 +5094,7 @@
         <v>20</v>
       </c>
       <c r="F67" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="G67" t="s">
         <v>22</v>
@@ -5077,16 +5106,16 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="J67" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="K67">
         <v>34176</v>
       </c>
       <c r="L67" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M67" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="N67" t="s">
         <v>26</v>
@@ -5095,7 +5124,7 @@
         <v>27</v>
       </c>
       <c r="P67" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q67" t="s">
         <v>20</v>
@@ -5103,13 +5132,13 @@
     </row>
     <row r="68" spans="1:17">
       <c r="A68" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B68" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C68" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D68" t="s">
         <v>20</v>
@@ -5118,7 +5147,7 @@
         <v>20</v>
       </c>
       <c r="F68" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G68" t="s">
         <v>22</v>
@@ -5130,16 +5159,16 @@
         <v>0.152</v>
       </c>
       <c r="J68" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="K68">
         <v>1276023</v>
       </c>
       <c r="L68" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M68" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="N68" t="s">
         <v>26</v>
@@ -5148,21 +5177,21 @@
         <v>27</v>
       </c>
       <c r="P68" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q68" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:17">
       <c r="A69" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D69" t="s">
         <v>20</v>
@@ -5171,7 +5200,7 @@
         <v>20</v>
       </c>
       <c r="F69" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G69" t="s">
         <v>22</v>
@@ -5183,16 +5212,16 @@
         <v>1.21</v>
       </c>
       <c r="J69" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="K69">
         <v>926</v>
       </c>
       <c r="L69" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="M69" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="N69" t="s">
         <v>26</v>
@@ -5201,7 +5230,7 @@
         <v>27</v>
       </c>
       <c r="P69" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="Q69" t="s">
         <v>20</v>
@@ -5209,22 +5238,16 @@
     </row>
     <row r="70" spans="1:17">
       <c r="A70" s="2" t="s">
-        <v>29</v>
+        <v>335</v>
       </c>
       <c r="B70" t="s">
-        <v>30</v>
+        <v>334</v>
       </c>
       <c r="C70" t="s">
-        <v>31</v>
-      </c>
-      <c r="D70" t="s">
-        <v>20</v>
-      </c>
-      <c r="E70" t="s">
-        <v>20</v>
+        <v>331</v>
       </c>
       <c r="F70" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G70" t="s">
         <v>22</v>
@@ -5233,19 +5256,19 @@
         <v>1</v>
       </c>
       <c r="I70">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="J70" t="s">
-        <v>33</v>
-      </c>
-      <c r="K70">
-        <v>1583</v>
+        <v>0.68</v>
+      </c>
+      <c r="J70" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="K70" s="18">
+        <v>1031</v>
       </c>
       <c r="L70" t="s">
-        <v>34</v>
+        <v>333</v>
       </c>
       <c r="M70" t="s">
-        <v>35</v>
+        <v>332</v>
       </c>
       <c r="N70" t="s">
         <v>26</v>
@@ -5254,41 +5277,96 @@
         <v>27</v>
       </c>
       <c r="P70" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>20</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17">
+      <c r="A71" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B71" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C71" t="s">
+        <v>336</v>
+      </c>
+      <c r="F71" t="s">
+        <v>29</v>
+      </c>
+      <c r="G71" t="s">
+        <v>22</v>
+      </c>
+      <c r="H71">
+        <v>2</v>
+      </c>
+      <c r="I71">
+        <v>0.11</v>
+      </c>
+      <c r="J71" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="K71" s="18">
+        <v>233568</v>
+      </c>
+      <c r="L71" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="M71" t="s">
+        <v>339</v>
+      </c>
+      <c r="N71" t="s">
+        <v>26</v>
+      </c>
+      <c r="O71" t="s">
+        <v>27</v>
+      </c>
+      <c r="P71" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="72" spans="1:17">
-      <c r="A72" s="14"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="3"/>
-      <c r="K72" s="3"/>
-      <c r="L72" s="3"/>
-      <c r="M72" s="3"/>
-    </row>
-    <row r="73" spans="1:17">
-      <c r="A73" s="14"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-      <c r="J73" s="3"/>
-      <c r="K73" s="3"/>
-      <c r="L73" s="3"/>
-      <c r="M73" s="3"/>
+      <c r="A72" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B72" t="s">
+        <v>341</v>
+      </c>
+      <c r="C72" t="s">
+        <v>340</v>
+      </c>
+      <c r="F72" t="s">
+        <v>270</v>
+      </c>
+      <c r="G72" t="s">
+        <v>22</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J72" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K72" s="18">
+        <v>31310</v>
+      </c>
+      <c r="L72" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="M72" t="s">
+        <v>344</v>
+      </c>
+      <c r="N72" t="s">
+        <v>26</v>
+      </c>
+      <c r="O72" t="s">
+        <v>27</v>
+      </c>
+      <c r="P72" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="74" spans="1:17">
       <c r="A74" s="14"/>
@@ -5305,80 +5383,110 @@
       <c r="L74" s="3"/>
       <c r="M74" s="3"/>
     </row>
-    <row r="76" spans="1:17" ht="56.25" customHeight="1">
-      <c r="A76" s="15" t="s">
+    <row r="75" spans="1:17">
+      <c r="A75" s="14"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+    </row>
+    <row r="76" spans="1:17">
+      <c r="A76" s="14"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+    </row>
+    <row r="78" spans="1:17" ht="56.25" customHeight="1">
+      <c r="A78" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78" s="6">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" ht="64.5" customHeight="1">
+      <c r="A79" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C79" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79" s="6">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" ht="27" customHeight="1"/>
+    <row r="81" spans="1:9" ht="43.9" customHeight="1">
+      <c r="A81" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="B81" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="H76">
+      <c r="C81" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9">
         <v>1</v>
       </c>
-      <c r="I76" s="6">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" ht="64.5" customHeight="1">
-      <c r="A77" s="16" t="s">
-        <v>327</v>
-      </c>
-      <c r="B77" s="5" t="s">
+      <c r="I81" s="10">
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="40.9" customHeight="1">
+      <c r="A82" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="B82" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="H77">
+      <c r="C82" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9">
         <v>1</v>
       </c>
-      <c r="I77" s="6">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" ht="27" customHeight="1"/>
-    <row r="79" spans="1:17" ht="43.9" customHeight="1">
-      <c r="A79" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9">
-        <v>1</v>
-      </c>
-      <c r="I79" s="10">
-        <v>64.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" ht="40.9" customHeight="1">
-      <c r="A80" s="17" t="s">
-        <v>334</v>
-      </c>
-      <c r="B80" s="11" t="s">
-        <v>333</v>
-      </c>
-      <c r="C80" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="D80" s="9"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9">
-        <v>1</v>
-      </c>
-      <c r="I80" s="10">
+      <c r="I82" s="10">
         <v>61.5</v>
       </c>
     </row>
@@ -5387,8 +5495,8 @@
     <sortCondition ref="M2:M80"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B76" r:id="rId1"/>
-    <hyperlink ref="B77" r:id="rId2"/>
+    <hyperlink ref="B78" r:id="rId1"/>
+    <hyperlink ref="B79" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
updated BOM for latest board revision
updated to include updates to current board rev
(ESP32 wifi module, and resistors for 7.0" tft if installed)
</commit_message>
<xml_diff>
--- a/BOM/T962A_Controller_TFT_BOM.xlsx
+++ b/BOM/T962A_Controller_TFT_BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="359">
   <si>
     <t>Manufacturer Part Number</t>
   </si>
@@ -1053,15 +1053,6 @@
     </r>
   </si>
   <si>
-    <t>NHD-5.0-800480MB-ATXL-CTP</t>
-  </si>
-  <si>
-    <t>http://www.newhavendisplay.com/nhd50800480mbatxlctp-p-9611.html</t>
-  </si>
-  <si>
-    <t>5.0" TFT w/mounting bracket</t>
-  </si>
-  <si>
     <t>https://www.newhavendisplay.com/nhd50800480tfatxlctp-p-6062.html</t>
   </si>
   <si>
@@ -1111,13 +1102,64 @@
   </si>
   <si>
     <t>BATTERY RETAINER COIN 20MM SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESP32-WROOM-32D </t>
+  </si>
+  <si>
+    <t>Espressif Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1904-1023-1-ND </t>
+  </si>
+  <si>
+    <t>2 Weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIFI MODULE 32MBITS SPI FLASH </t>
+  </si>
+  <si>
+    <t>P1.58KHCT-ND</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF1581V</t>
+  </si>
+  <si>
+    <t>Panasonic Electronic Component</t>
+  </si>
+  <si>
+    <t>RES SMD 1.58K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 47K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF4702V</t>
+  </si>
+  <si>
+    <t>P47.0KHCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.newhavendisplay.com/nhd70800480efasxnctp-p-9501.html</t>
+  </si>
+  <si>
+    <t>7.0" TFT w/NO bracket</t>
+  </si>
+  <si>
+    <t>NHD-7.0-800480EF-ASXN#-CTP</t>
+  </si>
+  <si>
+    <t>**** CHOOSE ONE OF THESE DEPENDING ON YOUR REGION VOLTAGE ***</t>
+  </si>
+  <si>
+    <t>***  CHOOSE 1 OF THESE, 5.0" OR 7.0" SCREEN ***</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1157,6 +1199,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1217,7 +1266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1231,12 +1280,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1260,6 +1303,9 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1554,10 +1600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q82"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="J83" sqref="J83:K86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1580,7 +1626,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -5238,13 +5284,13 @@
     </row>
     <row r="70" spans="1:17">
       <c r="A70" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B70" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C70" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F70" t="s">
         <v>29</v>
@@ -5261,14 +5307,14 @@
       <c r="J70" s="2">
         <v>0.68</v>
       </c>
-      <c r="K70" s="18">
+      <c r="K70" s="16">
         <v>1031</v>
       </c>
       <c r="L70" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="M70" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="N70" t="s">
         <v>26</v>
@@ -5282,13 +5328,13 @@
     </row>
     <row r="71" spans="1:17">
       <c r="A71" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="B71" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="B71" s="17" t="s">
         <v>215</v>
       </c>
       <c r="C71" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F71" t="s">
         <v>29</v>
@@ -5305,14 +5351,14 @@
       <c r="J71" s="2">
         <v>0.11</v>
       </c>
-      <c r="K71" s="18">
+      <c r="K71" s="16">
         <v>233568</v>
       </c>
-      <c r="L71" s="19" t="s">
-        <v>338</v>
+      <c r="L71" s="17" t="s">
+        <v>335</v>
       </c>
       <c r="M71" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N71" t="s">
         <v>26</v>
@@ -5326,13 +5372,13 @@
     </row>
     <row r="72" spans="1:17">
       <c r="A72" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B72" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C72" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F72" t="s">
         <v>270</v>
@@ -5349,57 +5395,159 @@
       <c r="J72" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K72" s="18">
+      <c r="K72" s="16">
         <v>31310</v>
       </c>
-      <c r="L72" s="19" t="s">
+      <c r="L72" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="M72" t="s">
+        <v>341</v>
+      </c>
+      <c r="N72" t="s">
+        <v>26</v>
+      </c>
+      <c r="O72" t="s">
+        <v>27</v>
+      </c>
+      <c r="P72" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17">
+      <c r="A73" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B73" t="s">
+        <v>349</v>
+      </c>
+      <c r="C73" t="s">
+        <v>353</v>
+      </c>
+      <c r="F73" t="s">
+        <v>29</v>
+      </c>
+      <c r="G73" t="s">
+        <v>22</v>
+      </c>
+      <c r="H73">
+        <v>10</v>
+      </c>
+      <c r="I73">
+        <v>0.65</v>
+      </c>
+      <c r="J73" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="K73" s="16">
+        <v>1277210</v>
+      </c>
+      <c r="L73" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="M73" t="s">
+        <v>351</v>
+      </c>
+      <c r="N73" t="s">
+        <v>26</v>
+      </c>
+      <c r="O73" t="s">
+        <v>27</v>
+      </c>
+      <c r="P73" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17">
+      <c r="A74" t="s">
+        <v>347</v>
+      </c>
+      <c r="B74" t="s">
+        <v>349</v>
+      </c>
+      <c r="C74" t="s">
+        <v>348</v>
+      </c>
+      <c r="F74" t="s">
+        <v>29</v>
+      </c>
+      <c r="G74" t="s">
+        <v>22</v>
+      </c>
+      <c r="H74">
+        <v>10</v>
+      </c>
+      <c r="I74">
+        <v>0.65</v>
+      </c>
+      <c r="J74" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="K74" s="16">
+        <v>76722</v>
+      </c>
+      <c r="L74" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="M74" t="s">
+        <v>350</v>
+      </c>
+      <c r="N74" t="s">
+        <v>26</v>
+      </c>
+      <c r="O74" t="s">
+        <v>27</v>
+      </c>
+      <c r="P74" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17">
+      <c r="A75" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B75" t="s">
         <v>343</v>
       </c>
-      <c r="M72" t="s">
+      <c r="C75" t="s">
         <v>344</v>
       </c>
-      <c r="N72" t="s">
-        <v>26</v>
-      </c>
-      <c r="O72" t="s">
-        <v>27</v>
-      </c>
-      <c r="P72" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17">
-      <c r="A74" s="14"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-      <c r="L74" s="3"/>
-      <c r="M74" s="3"/>
-    </row>
-    <row r="75" spans="1:17">
-      <c r="A75" s="14"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
-      <c r="J75" s="3"/>
-      <c r="K75" s="3"/>
-      <c r="L75" s="3"/>
-      <c r="M75" s="3"/>
+      <c r="F75" t="s">
+        <v>29</v>
+      </c>
+      <c r="G75" t="s">
+        <v>22</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>3.8</v>
+      </c>
+      <c r="J75" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="K75" s="16">
+        <v>7809</v>
+      </c>
+      <c r="L75" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="M75" t="s">
+        <v>346</v>
+      </c>
+      <c r="N75" t="s">
+        <v>26</v>
+      </c>
+      <c r="O75" t="s">
+        <v>27</v>
+      </c>
+      <c r="P75" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="76" spans="1:17">
-      <c r="A76" s="14"/>
+      <c r="A76" s="12"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
@@ -5413,90 +5561,144 @@
       <c r="L76" s="3"/>
       <c r="M76" s="3"/>
     </row>
-    <row r="78" spans="1:17" ht="56.25" customHeight="1">
-      <c r="A78" s="15" t="s">
+    <row r="77" spans="1:17">
+      <c r="A77" s="12"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+    </row>
+    <row r="78" spans="1:17">
+      <c r="A78" s="12"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+    </row>
+    <row r="80" spans="1:17" ht="56.25" customHeight="1">
+      <c r="A80" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B80" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C80" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="H78">
+      <c r="D80" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="E80" s="18"/>
+      <c r="H80">
         <v>1</v>
       </c>
-      <c r="I78" s="6">
+      <c r="I80" s="6">
         <v>1.4</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="64.5" customHeight="1">
-      <c r="A79" s="16" t="s">
+    <row r="81" spans="1:11" ht="64.5" customHeight="1">
+      <c r="A81" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B81" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="C81" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="H79">
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="H81">
         <v>1</v>
       </c>
-      <c r="I79" s="6">
+      <c r="I81" s="6">
         <v>1.4</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="27" customHeight="1"/>
-    <row r="81" spans="1:9" ht="43.9" customHeight="1">
-      <c r="A81" s="17" t="s">
+    <row r="82" spans="1:11" ht="27" customHeight="1"/>
+    <row r="83" spans="1:11" ht="40.9" customHeight="1">
+      <c r="A83" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="B83" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="B81" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="C81" s="8" t="s">
+      <c r="C83" s="10" t="s">
         <v>327</v>
       </c>
-      <c r="D81" s="9"/>
-      <c r="E81" s="9"/>
-      <c r="F81" s="9"/>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9">
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7">
         <v>1</v>
       </c>
-      <c r="I81" s="10">
-        <v>64.5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="40.9" customHeight="1">
-      <c r="A82" s="17" t="s">
-        <v>329</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="C82" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="D82" s="9"/>
-      <c r="E82" s="9"/>
-      <c r="F82" s="9"/>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9">
+      <c r="I83" s="8">
+        <v>61.5</v>
+      </c>
+      <c r="J83" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="K83" s="18"/>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="J84" s="18"/>
+      <c r="K84" s="18"/>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="J85" s="18"/>
+      <c r="K85" s="18"/>
+    </row>
+    <row r="86" spans="1:11" ht="31.5">
+      <c r="A86" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7">
         <v>1</v>
       </c>
-      <c r="I82" s="10">
-        <v>61.5</v>
-      </c>
+      <c r="I86" s="8">
+        <v>96.87</v>
+      </c>
+      <c r="J86" s="18"/>
+      <c r="K86" s="18"/>
     </row>
   </sheetData>
   <sortState ref="A2:Q80">
     <sortCondition ref="M2:M80"/>
   </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="D80:E81"/>
+    <mergeCell ref="J83:K86"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B78" r:id="rId1"/>
-    <hyperlink ref="B79" r:id="rId2"/>
+    <hyperlink ref="B80" r:id="rId1"/>
+    <hyperlink ref="B81" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>